<commit_message>
codigo super mega terminado
</commit_message>
<xml_diff>
--- a/writable/uploads/ssm_data.xlsx
+++ b/writable/uploads/ssm_data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="64">
   <si>
     <t>id</t>
   </si>
@@ -150,6 +150,63 @@
   </si>
   <si>
     <t>2023-08-13 22:55:28</t>
+  </si>
+  <si>
+    <t>000004</t>
+  </si>
+  <si>
+    <t>Conveyer2</t>
+  </si>
+  <si>
+    <t>josue</t>
+  </si>
+  <si>
+    <t>2023-08-13 23:44:18</t>
+  </si>
+  <si>
+    <t>2023-08-13 23:45:00</t>
+  </si>
+  <si>
+    <t>000005</t>
+  </si>
+  <si>
+    <t>inyeccion</t>
+  </si>
+  <si>
+    <t>probando</t>
+  </si>
+  <si>
+    <t>administracion</t>
+  </si>
+  <si>
+    <t>2023-08-13 23:51:57</t>
+  </si>
+  <si>
+    <t>2023-08-13 23:57:49</t>
+  </si>
+  <si>
+    <t>000006</t>
+  </si>
+  <si>
+    <t>prueba</t>
+  </si>
+  <si>
+    <t>2023-08-13 23:59:14</t>
+  </si>
+  <si>
+    <t>2023-08-13 23:59:47</t>
+  </si>
+  <si>
+    <t>000007</t>
+  </si>
+  <si>
+    <t>2023-08-09</t>
+  </si>
+  <si>
+    <t>2023-08-14 00:00:57</t>
+  </si>
+  <si>
+    <t>2023-08-14 00:01:19</t>
   </si>
 </sst>
 </file>
@@ -521,10 +578,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A4" sqref="A4:N4"/>
+      <selection activeCell="A8" sqref="A8:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -721,6 +778,182 @@
         <v>44</v>
       </c>
     </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="2">
+        <v>123456</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1234556</v>
+      </c>
+      <c r="L5" s="2">
+        <v>98765443</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="2">
+        <v>123456</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2143545</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1456778</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1234556</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1456778</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="2">
+        <v>413251</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1234556</v>
+      </c>
+      <c r="L8" s="2">
+        <v>98765443</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>